<commit_message>
produces prevalence in all surveys, including 95% CIs. Inputs allowed to be missing
</commit_message>
<xml_diff>
--- a/inst/extdata/prevalence_tests/correct_01.xlsx
+++ b/inst/extdata/prevalence_tests/correct_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rverity/Dropbox/Bob/Work/My Programs/Mapping/STAVE/inst/extdata/prevalence_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6EFD39-AB8D-7945-8392-70427E273A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0778DBE5-6061-A140-B8CE-9CDE320E6C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1120" windowWidth="31520" windowHeight="18700" activeTab="3" xr2:uid="{A4E9C168-401F-F34B-85A4-C504E7A73195}"/>
   </bookViews>
@@ -162,10 +162,10 @@
     <t>crt:72:A</t>
   </si>
   <si>
-    <t>crt:72_73_74:C|A_V|A_I</t>
-  </si>
-  <si>
     <t>crt:72_73_74:C|A|D_V|A|D_I</t>
+  </si>
+  <si>
+    <t>crt:72_73_74:C/A_V/A_I</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,7 +787,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -801,7 +801,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>

</xml_diff>

<commit_message>
changed IDs to lowercase id, ammended and tidied all structural checks, some work on pkgdown vignettes
</commit_message>
<xml_diff>
--- a/inst/extdata/prevalence_tests/correct_01.xlsx
+++ b/inst/extdata/prevalence_tests/correct_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rverity/Dropbox/Bob/Work/My Programs/Mapping/STAVE/inst/extdata/prevalence_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0778DBE5-6061-A140-B8CE-9CDE320E6C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12FECB-716F-5C4E-A8F9-A26457C85650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1120" windowWidth="31520" windowHeight="18700" activeTab="3" xr2:uid="{A4E9C168-401F-F34B-85A4-C504E7A73195}"/>
+    <workbookView xWindow="1380" yWindow="1120" windowWidth="31520" windowHeight="18700" activeTab="4" xr2:uid="{A4E9C168-401F-F34B-85A4-C504E7A73195}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>study_ID</t>
-  </si>
-  <si>
     <t>study_name</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>first study</t>
   </si>
   <si>
-    <t>survey_ID</t>
-  </si>
-  <si>
     <t>study_key</t>
   </si>
   <si>
@@ -90,12 +84,6 @@
     <t>site_name</t>
   </si>
   <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
     <t>spatial_notes</t>
   </si>
   <si>
@@ -166,6 +154,18 @@
   </si>
   <si>
     <t>crt:72_73_74:C/A_V/A_I</t>
+  </si>
+  <si>
+    <t>study_id</t>
+  </si>
+  <si>
+    <t>survey_id</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +583,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,42 +593,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
       <c r="E2">
         <v>2024</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -644,7 +644,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,51 +654,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -707,19 +707,19 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -731,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E51D5F-A46A-0B42-A5D0-47D275C37629}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -742,24 +742,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -770,10 +770,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -798,10 +798,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -812,10 +812,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -848,26 +848,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FD02AD-7538-844E-8161-FED3057DF0A4}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>0</v>

</xml_diff>